<commit_message>
stable server build without research
</commit_message>
<xml_diff>
--- a/sources/tables/companies.xlsx
+++ b/sources/tables/companies.xlsx
@@ -671,12 +671,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1 282 483,7</t>
+          <t>1 259 958,7</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1 419 486,1</t>
+          <t>1 399 765,6</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>599 530,7</t>
+          <t>590 999,6</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>698 254,4</t>
+          <t>689 156,7</t>
         </is>
       </c>
     </row>
@@ -741,12 +741,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>525 961,8</t>
+          <t>517 430,7</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>623 067,1</t>
+          <t>613 969,4</t>
         </is>
       </c>
     </row>
@@ -776,12 +776,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>336 782,4</t>
+          <t>325 349,4</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>440 257,4</t>
+          <t>428 181,2</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2 203</t>
+          <t>2 128</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2 880</t>
+          <t>2 801</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>46,7  %</t>
+          <t>46,9  %</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>41,0  %</t>
+          <t>41,1  %</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -967,12 +967,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>26,3  %</t>
+          <t>25,8  %</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>31,0  %</t>
+          <t>30,6  %</t>
         </is>
       </c>
     </row>
@@ -1078,12 +1078,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5.1</t>
         </is>
       </c>
     </row>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1123,12 +1123,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.9</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1158,12 +1158,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
@@ -1244,12 +1244,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10,98  %</t>
+          <t>9,03  %</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10,68  %</t>
+          <t>11,10  %</t>
         </is>
       </c>
     </row>
@@ -1279,12 +1279,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-0,13  %</t>
+          <t>-1,55  %</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>16,47  %</t>
+          <t>16,61  %</t>
         </is>
       </c>
     </row>
@@ -1314,12 +1314,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-7  %</t>
+          <t>-11  %</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>31  %</t>
+          <t>32  %</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>12.6</t>
+          <t>12.7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2777,7 +2777,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>2.8</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -2827,17 +2827,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-180.6</t>
+          <t>-180.9</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.3</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3486,27 +3486,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>3.8</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>3.7</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>3.6</t>
         </is>
       </c>
     </row>
@@ -3521,27 +3521,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15.3</t>
+          <t>15.7</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>6.3</t>
         </is>
       </c>
     </row>
@@ -3556,27 +3556,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>5.5</t>
         </is>
       </c>
     </row>
@@ -4718,27 +4718,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.9</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.6</t>
         </is>
       </c>
     </row>
@@ -4753,27 +4753,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>13.6</t>
+          <t>14.0</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.5</t>
         </is>
       </c>
     </row>
@@ -4788,27 +4788,27 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.6</t>
         </is>
       </c>
     </row>

</xml_diff>